<commit_message>
New: Detect redundant answer choices; Refactoring: GetMetadataOfQuestions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scep\Documents\UiPath\zid-moodle-exam-checker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA44602-1A6E-41AB-81BE-22809A98B6B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F00450-9D61-4276-91A2-A0BD570DBCD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -229,9 +229,6 @@
   </si>
   <si>
     <t>Empty, if all questions shall be processed. A date, if only questions modified since this date shall be processed</t>
-  </si>
-  <si>
-    <t>68</t>
   </si>
 </sst>
 </file>
@@ -613,7 +610,7 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -684,9 +681,7 @@
       <c r="A4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="B4" s="6"/>
       <c r="C4" s="3" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
New: Get Quiz Metadata from Quiz Edit Page; Documentation started
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scep\Documents\UiPath\zid-moodle-exam-checker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F00450-9D61-4276-91A2-A0BD570DBCD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623D924A-E5D3-42D9-B58C-6345B111334E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Empty, if all questions shall be processed. A date, if only questions modified since this date shall be processed</t>
+  </si>
+  <si>
+    <t>2-6</t>
   </si>
 </sst>
 </file>
@@ -610,7 +613,7 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -681,7 +684,9 @@
       <c r="A4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Improve: React on Pop up to leave page; Temporary Bugfix: img with src='data:...'
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scep\Documents\UiPath\zid-moodle-exam-checker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623D924A-E5D3-42D9-B58C-6345B111334E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F20B81-43E7-45AA-B024-FDE3F00E1A17}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -231,7 +231,7 @@
     <t>Empty, if all questions shall be processed. A date, if only questions modified since this date shall be processed</t>
   </si>
   <si>
-    <t>2-6</t>
+    <t>82-118</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Adaption to new Moodle Version
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scep\Documents\UiPath\zid-moodle-exam-checker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BAC35E-A433-4354-A4FD-324A82B14CAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5C7431-E44C-4A2A-99C0-4FF710EB9FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
     <t>Empty, if all questions shall be processed. A date, if only questions modified since this date shall be processed</t>
   </si>
   <si>
-    <t>57-58</t>
+    <t>72</t>
   </si>
 </sst>
 </file>
@@ -613,7 +613,7 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2923,6 +2923,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3976,5 +3977,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Inserted Delay because of H_RESULT error
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scep\Documents\UiPath\zid-moodle-exam-checker\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5C7431-E44C-4A2A-99C0-4FF710EB9FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D0E333-1441-4D37-9189-CA69A2015341}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -229,9 +229,6 @@
   </si>
   <si>
     <t>Empty, if all questions shall be processed. A date, if only questions modified since this date shall be processed</t>
-  </si>
-  <si>
-    <t>72</t>
   </si>
 </sst>
 </file>
@@ -613,7 +610,7 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -684,9 +681,7 @@
       <c r="A4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="B4" s="6"/>
       <c r="C4" s="3" t="s">
         <v>63</v>
       </c>

</xml_diff>